<commit_message>
Added session 1 and 2 edits and session 4 for review
</commit_message>
<xml_diff>
--- a/2022_dplyr_version/data/Sampling_frames.xlsx
+++ b/2022_dplyr_version/data/Sampling_frames.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymi\Documents\MyDocs\07_Consults\EPIET_RAS_R_updates\2022_RAS_R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amymi\Documents\MyDocs\07_Consults\EPIET_RAS_R_updates\RapidAssessmentSurveys\2022_dplyr_version\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7267B66-6D73-43CB-8F6C-8C3649CE7B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D5D36-6F99-4FF2-B355-87F039B3B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20408" windowHeight="13065" activeTab="3" xr2:uid="{15C14FEE-6E7E-4B49-817D-558E93018195}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20408" windowHeight="13065" activeTab="4" xr2:uid="{15C14FEE-6E7E-4B49-817D-558E93018195}"/>
   </bookViews>
   <sheets>
     <sheet name="table1_2" sheetId="1" r:id="rId1"/>
     <sheet name="table1_3" sheetId="3" r:id="rId2"/>
     <sheet name="table1_5" sheetId="2" r:id="rId3"/>
     <sheet name="table2_1" sheetId="4" r:id="rId4"/>
+    <sheet name="table4_2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="231">
   <si>
     <t>Urban</t>
   </si>
@@ -692,13 +693,52 @@
   </si>
   <si>
     <t>Student_pop</t>
+  </si>
+  <si>
+    <t>Stratum_id</t>
+  </si>
+  <si>
+    <t>Stratum_name</t>
+  </si>
+  <si>
+    <t>Area_type</t>
+  </si>
+  <si>
+    <t>Total_pupils</t>
+  </si>
+  <si>
+    <t>Selected_pupils</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>Ipiros</t>
+  </si>
+  <si>
+    <t>Aegean</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Attica</t>
+  </si>
+  <si>
+    <t>Sterea</t>
+  </si>
+  <si>
+    <t>Thrace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +767,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -748,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -776,6 +822,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2907,7 +2962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52BA39B-59BB-4520-8557-64F5ED18EAFA}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -2980,4 +3035,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3221CAF8-7C2E-49AA-BF3E-1A0DAAB52FBC}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.06640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.53125" customWidth="1"/>
+    <col min="3" max="3" width="12.265625" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.265625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="13">
+        <v>3282</v>
+      </c>
+      <c r="E2" s="9">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1773</v>
+      </c>
+      <c r="E3" s="9">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="14">
+        <v>8609</v>
+      </c>
+      <c r="E4" s="9">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3609</v>
+      </c>
+      <c r="E5" s="9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="14">
+        <v>24311</v>
+      </c>
+      <c r="E6" s="9">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="14">
+        <v>6734</v>
+      </c>
+      <c r="E7" s="9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="14">
+        <v>30345</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="14">
+        <v>12928</v>
+      </c>
+      <c r="E9" s="9">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="14">
+        <v>4813</v>
+      </c>
+      <c r="E10" s="9">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" s="14">
+        <v>3069</v>
+      </c>
+      <c r="E11" s="9">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1132</v>
+      </c>
+      <c r="E12" s="9">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>